<commit_message>
Se actualiza codigo hasta Recibo
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sispmunoz\Documents\Gestoria\gestoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E73037-6ADF-4E4D-8C2B-09BCAFFD3116}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51B87C8-4827-4F09-82A8-14B805969B03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>admmartha</t>
   </si>
@@ -123,7 +123,55 @@
     <t>Documento Permiso</t>
   </si>
   <si>
-    <t>folio, fecha, fechaVigencia, tipoDocumento, rfc, razonSocial, responsiva, documento);</t>
+    <t>Fecha Vigencia:</t>
+  </si>
+  <si>
+    <t>Tipo Documento:</t>
+  </si>
+  <si>
+    <t>RFC:</t>
+  </si>
+  <si>
+    <t>Razon Social:</t>
+  </si>
+  <si>
+    <t>Responsiva:</t>
+  </si>
+  <si>
+    <t>Documento:</t>
+  </si>
+  <si>
+    <t>28-09-2020</t>
+  </si>
+  <si>
+    <t>ORIGINAL</t>
+  </si>
+  <si>
+    <t>MUCP880820N50</t>
+  </si>
+  <si>
+    <t>Razon Social Prueba</t>
+  </si>
+  <si>
+    <t>Responsiva</t>
+  </si>
+  <si>
+    <t>C:\\Users\\sispmunoz\\Desktop\\DocumentoPermiso.pdf</t>
+  </si>
+  <si>
+    <t>Recibo</t>
+  </si>
+  <si>
+    <t>Importe:</t>
+  </si>
+  <si>
+    <t>Metodo Pago:</t>
+  </si>
+  <si>
+    <t>R001</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -447,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C29"/>
+  <dimension ref="A2:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,8 +651,112 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>32</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza el código 11112020
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sispmunoz\Documents\Gestoria\gestoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51B87C8-4827-4F09-82A8-14B805969B03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DFFA3A-6845-45A6-B585-7E9EC40D1958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>admmartha</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Tipo de Permiso:</t>
   </si>
   <si>
-    <t>ANUENCIA DE FUNCIONAMIENTO</t>
-  </si>
-  <si>
     <t>Documento Inicio de Tramite</t>
   </si>
   <si>
@@ -172,6 +169,36 @@
   </si>
   <si>
     <t>1000</t>
+  </si>
+  <si>
+    <t>Factura</t>
+  </si>
+  <si>
+    <t>F001</t>
+  </si>
+  <si>
+    <t>Observaciones:</t>
+  </si>
+  <si>
+    <t>Observaciones prueba</t>
+  </si>
+  <si>
+    <t>INGRESADO</t>
+  </si>
+  <si>
+    <t>Opciones tabla permisos:</t>
+  </si>
+  <si>
+    <t>detalle</t>
+  </si>
+  <si>
+    <t>editar</t>
+  </si>
+  <si>
+    <t>eliminar</t>
+  </si>
+  <si>
+    <t>ALTA DE HACIENDA</t>
   </si>
 </sst>
 </file>
@@ -207,13 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C43"/>
+  <dimension ref="A2:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,164 +635,254 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A56:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se actualiza el código 12112020
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sispmunoz\Documents\Gestoria\gestoria\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>admmartha</t>
   </si>
@@ -205,6 +205,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,8 +534,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="58.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>